<commit_message>
Update salesman has no contract
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_SUMMARY_TEMPLATE_NO_ARGEEMENT.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_SUMMARY_TEMPLATE_NO_ARGEEMENT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8100" windowWidth="28770" windowHeight="6885"/>
+    <workbookView xWindow="0" yWindow="8550" windowWidth="28770" windowHeight="6885"/>
   </bookViews>
   <sheets>
     <sheet name="AR SUMMARY" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Debit Amount</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>{ServiceName}</t>
+  </si>
+  <si>
+    <t>{ArSalesmanName}</t>
+  </si>
+  <si>
+    <t>Salesman</t>
   </si>
 </sst>
 </file>
@@ -566,13 +572,13 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,8 +593,7 @@
     <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30" style="1" customWidth="1"/>
+    <col min="11" max="13" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" customWidth="1"/>
@@ -609,7 +614,7 @@
     <col min="32" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -646,8 +651,11 @@
       <c r="L1" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="M1" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -684,8 +692,11 @@
       <c r="L2" s="6">
         <v>12</v>
       </c>
+      <c r="M2" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -722,23 +733,26 @@
       <c r="L3" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="M3" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>

</xml_diff>